<commit_message>
Pushing updates to ERP Tank mating rail had typo of MCh instead of MCH
</commit_message>
<xml_diff>
--- a/OpsAndMats/8025044.xlsx
+++ b/OpsAndMats/8025044.xlsx
@@ -239,7 +239,7 @@
     <t>9816011</t>
   </si>
   <si>
-    <t>3704043</t>
+    <t>3704301</t>
   </si>
   <si>
     <t>3704047</t>
@@ -260,7 +260,7 @@
     <t>Zinc Plating</t>
   </si>
   <si>
-    <t>3/4-10 steel threaded rod</t>
+    <t xml:space="preserve">3/4-10 steel threaded rod, </t>
   </si>
   <si>
     <t>1"-8 steel threaded rod</t>

</xml_diff>